<commit_message>
Updated the notes 3/19/2020 evening
</commit_message>
<xml_diff>
--- a/Work Blockchain Notes.xlsx
+++ b/Work Blockchain Notes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Work\blockchaining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594108CA-5478-41B1-92BF-7714E279FA9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B1AC1D-1ABE-4922-B81A-E363F4F02C73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43935" yWindow="9030" windowWidth="18435" windowHeight="9765" xr2:uid="{BDE38765-44BC-5F4C-A678-8771D11B51DC}"/>
+    <workbookView xWindow="20796" yWindow="7044" windowWidth="18432" windowHeight="9768" xr2:uid="{BDE38765-44BC-5F4C-A678-8771D11B51DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
   <si>
     <t>Abstract</t>
   </si>
@@ -222,9 +222,6 @@
     <t>I've come to realize that the only things this apper can give me are papers from prior to 2016</t>
   </si>
   <si>
-    <t>Making Sense of Blockchain Applications: A Typology for HCI</t>
-  </si>
-  <si>
     <t>https://dl.acm.org/doi/pdf/10.1145/3173574.3174032</t>
   </si>
   <si>
@@ -234,7 +231,25 @@
     <t>https://static1.squarespace.com/static/563240cae4b056714fc21c26/t/5bc13eb5b208fcee0e8ad937/1539391159544/LacityMISQEBlockchains2018.pdf</t>
   </si>
   <si>
-    <t>Addressing Key Challenges to Making Enterprise Blockchain Applications a Reality</t>
+    <t>Not sure this will help us</t>
+  </si>
+  <si>
+    <t>Addressing Key Challenges to Making Enterprise Blockchain Applications a Reality (2018)</t>
+  </si>
+  <si>
+    <t>Making Sense of Blockchain Applications: A Typology for HCI (2018)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=jxLkbJozKbY</t>
+  </si>
+  <si>
+    <t>What is Ethereum? A Beginner's Explanation in Plain English</t>
+  </si>
+  <si>
+    <t>This is just a YouTube video I watched on my own time, but I figured I'd throw it in here for fun. It goes over the Ethereum platform, and also explains Blockchain again. One thing I really liked was when he said "Blockchain is to Bitcoin and the Internet is to Email." He goes to explain that Ethereum was created as a platform to create decentralized applications, the same way blockchain came about in order to make a decentralized currency, Bitcoin. Ethereum is a network of independent computers running Decentralized Apps</t>
+  </si>
+  <si>
+    <t>I mean. I doubt we can use this in our paper, but it was a good intro to knowing about a platform used for making decentralized applications</t>
   </si>
 </sst>
 </file>
@@ -674,7 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -715,6 +730,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -784,6 +802,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -820,29 +862,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -855,42 +909,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1207,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659183C7-6FCE-A94E-ACE3-15A5F17A3D83}">
-  <dimension ref="A1:H117"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93:G93"/>
+    <sheetView tabSelected="1" topLeftCell="B110" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113:G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="18"/>
@@ -1219,396 +1237,396 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:7" ht="106.05" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="1:7" ht="118.05" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="48"/>
     </row>
     <row r="5" spans="1:7" ht="90" customHeight="1">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="51"/>
     </row>
     <row r="6" spans="1:7" ht="91.05" customHeight="1">
-      <c r="A6" s="26"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="45"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="54"/>
     </row>
     <row r="7" spans="1:7" ht="91.05" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="24"/>
     </row>
     <row r="8" spans="1:7" ht="91.05" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
     </row>
     <row r="9" spans="1:7" ht="106.05" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
     </row>
     <row r="10" spans="1:7" ht="105" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:7" ht="28.05" customHeight="1"/>
     <row r="12" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:7" ht="109.05" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="24"/>
     </row>
     <row r="15" spans="1:7" ht="109.05" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="42"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
     </row>
     <row r="17" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A17" s="26"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="54"/>
     </row>
     <row r="18" spans="1:7" ht="109.05" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
     </row>
     <row r="19" spans="1:7" ht="109.05" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
     </row>
     <row r="20" spans="1:7" ht="28.05" customHeight="1"/>
     <row r="21" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
     </row>
     <row r="23" spans="1:7" ht="109.05" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="24"/>
     </row>
     <row r="24" spans="1:7" ht="109.05" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="66"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="63"/>
     </row>
     <row r="25" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="67" t="s">
+      <c r="B25" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="69"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="66"/>
     </row>
     <row r="26" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="70"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="72"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="69"/>
     </row>
     <row r="27" spans="1:7" ht="109.05" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
     </row>
     <row r="28" spans="1:7" ht="21" customHeight="1" thickBot="1"/>
     <row r="29" spans="1:7" ht="28.05" customHeight="1" thickTop="1">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="48"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="57"/>
     </row>
     <row r="30" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A30" s="55" t="s">
+      <c r="A30" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="56"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="45"/>
     </row>
     <row r="31" spans="1:7" ht="109.05" customHeight="1">
       <c r="A31" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="57"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="70"/>
     </row>
     <row r="32" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="49"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="38"/>
     </row>
     <row r="33" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A33" s="53"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="50"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="39"/>
     </row>
     <row r="34" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A34" s="53"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="50"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="39"/>
     </row>
     <row r="35" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A35" s="54"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="51"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="40"/>
     </row>
     <row r="36" spans="1:7" ht="109.05" customHeight="1" thickBot="1">
       <c r="A36" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="58" t="s">
+      <c r="B36" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="60"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="73"/>
     </row>
     <row r="37" spans="1:7" ht="42" customHeight="1" thickTop="1">
       <c r="A37" s="8"/>
@@ -1620,92 +1638,92 @@
       <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="20"/>
     </row>
     <row r="39" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="20"/>
     </row>
     <row r="40" spans="1:7" ht="109.05" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="24"/>
     </row>
     <row r="41" spans="1:7" ht="49.95" customHeight="1">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="62"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="62"/>
-      <c r="G41" s="63"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="60"/>
     </row>
     <row r="42" spans="1:7" ht="49.95" customHeight="1">
-      <c r="A42" s="25"/>
-      <c r="B42" s="61"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="63"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="60"/>
     </row>
     <row r="43" spans="1:7" ht="49.95" customHeight="1">
-      <c r="A43" s="25"/>
-      <c r="B43" s="61"/>
-      <c r="C43" s="62"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="62"/>
-      <c r="F43" s="62"/>
-      <c r="G43" s="63"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="60"/>
     </row>
     <row r="44" spans="1:7" ht="49.95" customHeight="1">
-      <c r="A44" s="26"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="45"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="54"/>
     </row>
     <row r="45" spans="1:7" ht="109.05" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="17"/>
     </row>
     <row r="46" spans="1:7" ht="28.05" customHeight="1">
       <c r="A46" s="4"/>
@@ -1717,92 +1735,92 @@
       <c r="G46" s="6"/>
     </row>
     <row r="47" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="20"/>
     </row>
     <row r="48" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A48" s="20" t="s">
+      <c r="A48" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="20"/>
     </row>
     <row r="49" spans="1:7" ht="109.05" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="24"/>
     </row>
     <row r="50" spans="1:7" ht="64.95" customHeight="1">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="27" t="s">
+      <c r="B50" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="30"/>
     </row>
     <row r="51" spans="1:7" ht="64.95" customHeight="1">
-      <c r="A51" s="25"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="32"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="33"/>
     </row>
     <row r="52" spans="1:7" ht="64.95" customHeight="1">
-      <c r="A52" s="25"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="32"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="33"/>
     </row>
     <row r="53" spans="1:7" ht="64.95" customHeight="1">
-      <c r="A53" s="26"/>
-      <c r="B53" s="33"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="35"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="36"/>
     </row>
     <row r="54" spans="1:7" ht="109.05" customHeight="1">
       <c r="A54" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" ht="28.95" customHeight="1">
       <c r="A55" s="13"/>
@@ -1814,593 +1832,565 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="19"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="20"/>
     </row>
     <row r="57" spans="1:7" ht="58.95" customHeight="1">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="19"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="20"/>
     </row>
     <row r="58" spans="1:7" ht="109.05" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="24"/>
     </row>
     <row r="59" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A59" s="24" t="s">
+      <c r="A59" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B59" s="27"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="28"/>
-      <c r="F59" s="28"/>
-      <c r="G59" s="29"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="30"/>
     </row>
     <row r="60" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A60" s="25"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="32"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="33"/>
     </row>
     <row r="61" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A61" s="25"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="31"/>
-      <c r="F61" s="31"/>
-      <c r="G61" s="32"/>
+      <c r="A61" s="26"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="33"/>
     </row>
     <row r="62" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A62" s="26"/>
-      <c r="B62" s="33"/>
-      <c r="C62" s="34"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="35"/>
+      <c r="A62" s="27"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="36"/>
     </row>
     <row r="63" spans="1:7" ht="109.05" customHeight="1">
       <c r="A63" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="17"/>
     </row>
     <row r="65" spans="1:8" ht="28.05" customHeight="1">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="19"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="20"/>
     </row>
     <row r="66" spans="1:8" ht="28.05" customHeight="1">
-      <c r="A66" s="20" t="s">
+      <c r="A66" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="19"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="20"/>
     </row>
     <row r="67" spans="1:8" ht="130.19999999999999" customHeight="1">
       <c r="A67" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B67" s="21" t="s">
+      <c r="B67" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C67" s="22"/>
-      <c r="D67" s="22"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="22"/>
-      <c r="G67" s="23"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="24"/>
     </row>
     <row r="68" spans="1:8" ht="109.05" customHeight="1">
-      <c r="A68" s="24" t="s">
+      <c r="A68" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="40" t="s">
+      <c r="B68" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C68" s="41"/>
-      <c r="D68" s="41"/>
-      <c r="E68" s="41"/>
-      <c r="F68" s="41"/>
-      <c r="G68" s="42"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="50"/>
+      <c r="G68" s="51"/>
     </row>
     <row r="69" spans="1:8" ht="109.05" customHeight="1">
-      <c r="A69" s="25"/>
-      <c r="B69" s="61"/>
-      <c r="C69" s="62"/>
-      <c r="D69" s="62"/>
-      <c r="E69" s="62"/>
-      <c r="F69" s="62"/>
-      <c r="G69" s="63"/>
+      <c r="A69" s="26"/>
+      <c r="B69" s="58"/>
+      <c r="C69" s="59"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="59"/>
+      <c r="F69" s="59"/>
+      <c r="G69" s="60"/>
     </row>
     <row r="70" spans="1:8" ht="109.05" customHeight="1">
-      <c r="A70" s="25"/>
-      <c r="B70" s="61"/>
-      <c r="C70" s="62"/>
-      <c r="D70" s="62"/>
-      <c r="E70" s="62"/>
-      <c r="F70" s="62"/>
-      <c r="G70" s="63"/>
+      <c r="A70" s="26"/>
+      <c r="B70" s="58"/>
+      <c r="C70" s="59"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="59"/>
+      <c r="F70" s="59"/>
+      <c r="G70" s="60"/>
     </row>
     <row r="71" spans="1:8" ht="109.05" customHeight="1">
-      <c r="A71" s="26"/>
-      <c r="B71" s="43"/>
-      <c r="C71" s="44"/>
-      <c r="D71" s="44"/>
-      <c r="E71" s="44"/>
-      <c r="F71" s="44"/>
-      <c r="G71" s="45"/>
+      <c r="A71" s="27"/>
+      <c r="B71" s="52"/>
+      <c r="C71" s="53"/>
+      <c r="D71" s="53"/>
+      <c r="E71" s="53"/>
+      <c r="F71" s="53"/>
+      <c r="G71" s="54"/>
     </row>
     <row r="72" spans="1:8" ht="109.05" customHeight="1">
       <c r="A72" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="15"/>
-      <c r="F72" s="15"/>
-      <c r="G72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="17"/>
     </row>
     <row r="74" spans="1:8" ht="28.05" customHeight="1">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="36" t="s">
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="20"/>
+      <c r="H74" s="37" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="28.05" customHeight="1">
-      <c r="A75" s="20" t="s">
+      <c r="A75" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="19"/>
-      <c r="H75" s="36"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="20"/>
+      <c r="H75" s="37"/>
     </row>
     <row r="76" spans="1:8" ht="109.05" customHeight="1">
       <c r="A76" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B76" s="21"/>
-      <c r="C76" s="22"/>
-      <c r="D76" s="22"/>
-      <c r="E76" s="22"/>
-      <c r="F76" s="22"/>
-      <c r="G76" s="23"/>
+      <c r="B76" s="22"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="24"/>
     </row>
     <row r="77" spans="1:8" ht="109.05" customHeight="1">
-      <c r="A77" s="24" t="s">
+      <c r="A77" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B77" s="27"/>
-      <c r="C77" s="28"/>
-      <c r="D77" s="28"/>
-      <c r="E77" s="28"/>
-      <c r="F77" s="28"/>
-      <c r="G77" s="29"/>
+      <c r="B77" s="28"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="30"/>
     </row>
     <row r="78" spans="1:8" ht="109.05" customHeight="1">
-      <c r="A78" s="25"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="31"/>
-      <c r="F78" s="31"/>
-      <c r="G78" s="32"/>
+      <c r="A78" s="26"/>
+      <c r="B78" s="31"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="32"/>
+      <c r="F78" s="32"/>
+      <c r="G78" s="33"/>
     </row>
     <row r="79" spans="1:8" ht="109.05" customHeight="1">
-      <c r="A79" s="25"/>
-      <c r="B79" s="30"/>
-      <c r="C79" s="31"/>
-      <c r="D79" s="31"/>
-      <c r="E79" s="31"/>
-      <c r="F79" s="31"/>
-      <c r="G79" s="32"/>
+      <c r="A79" s="26"/>
+      <c r="B79" s="31"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="32"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="33"/>
     </row>
     <row r="80" spans="1:8" ht="109.05" customHeight="1">
-      <c r="A80" s="26"/>
-      <c r="B80" s="33"/>
-      <c r="C80" s="34"/>
-      <c r="D80" s="34"/>
-      <c r="E80" s="34"/>
-      <c r="F80" s="34"/>
-      <c r="G80" s="35"/>
+      <c r="A80" s="27"/>
+      <c r="B80" s="34"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="35"/>
+      <c r="E80" s="35"/>
+      <c r="F80" s="35"/>
+      <c r="G80" s="36"/>
     </row>
     <row r="81" spans="1:7" ht="109.05" customHeight="1">
       <c r="A81" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B81" s="14"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="15"/>
-      <c r="G81" s="16"/>
+      <c r="B81" s="15"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="17"/>
     </row>
     <row r="83" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B83" s="18"/>
-      <c r="C83" s="18"/>
-      <c r="D83" s="18"/>
-      <c r="E83" s="18"/>
-      <c r="F83" s="18"/>
-      <c r="G83" s="19"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="20"/>
     </row>
     <row r="84" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A84" s="20" t="s">
+      <c r="A84" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B84" s="18"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="18"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="19"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="19"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="19"/>
+      <c r="G84" s="20"/>
     </row>
     <row r="85" spans="1:7" ht="109.05" customHeight="1">
       <c r="A85" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B85" s="21"/>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="22"/>
-      <c r="G85" s="23"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="23"/>
+      <c r="F85" s="23"/>
+      <c r="G85" s="24"/>
     </row>
     <row r="86" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A86" s="24" t="s">
+      <c r="A86" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B86" s="27"/>
-      <c r="C86" s="28"/>
-      <c r="D86" s="28"/>
-      <c r="E86" s="28"/>
-      <c r="F86" s="28"/>
-      <c r="G86" s="29"/>
+      <c r="B86" s="28"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="29"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29"/>
+      <c r="G86" s="30"/>
     </row>
     <row r="87" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A87" s="25"/>
-      <c r="B87" s="30"/>
-      <c r="C87" s="31"/>
-      <c r="D87" s="31"/>
-      <c r="E87" s="31"/>
-      <c r="F87" s="31"/>
-      <c r="G87" s="32"/>
+      <c r="A87" s="26"/>
+      <c r="B87" s="31"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="32"/>
+      <c r="G87" s="33"/>
     </row>
     <row r="88" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A88" s="25"/>
-      <c r="B88" s="30"/>
-      <c r="C88" s="31"/>
-      <c r="D88" s="31"/>
-      <c r="E88" s="31"/>
-      <c r="F88" s="31"/>
-      <c r="G88" s="32"/>
+      <c r="A88" s="26"/>
+      <c r="B88" s="31"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="32"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="32"/>
+      <c r="G88" s="33"/>
     </row>
     <row r="89" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A89" s="26"/>
-      <c r="B89" s="33"/>
-      <c r="C89" s="34"/>
-      <c r="D89" s="34"/>
-      <c r="E89" s="34"/>
-      <c r="F89" s="34"/>
-      <c r="G89" s="35"/>
+      <c r="A89" s="27"/>
+      <c r="B89" s="34"/>
+      <c r="C89" s="35"/>
+      <c r="D89" s="35"/>
+      <c r="E89" s="35"/>
+      <c r="F89" s="35"/>
+      <c r="G89" s="36"/>
     </row>
     <row r="90" spans="1:7" ht="109.05" customHeight="1">
       <c r="A90" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B90" s="14"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="15"/>
-      <c r="G90" s="16"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="16"/>
+      <c r="E90" s="16"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="17"/>
     </row>
     <row r="92" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A92" s="17" t="s">
+      <c r="A92" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="20"/>
+    </row>
+    <row r="93" spans="1:7" ht="28.05" customHeight="1">
+      <c r="A93" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B92" s="18"/>
-      <c r="C92" s="18"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="18"/>
-      <c r="F92" s="18"/>
-      <c r="G92" s="19"/>
-    </row>
-    <row r="93" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A93" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B93" s="18"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="18"/>
-      <c r="E93" s="18"/>
-      <c r="F93" s="18"/>
-      <c r="G93" s="19"/>
+      <c r="B93" s="19"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
+      <c r="G93" s="20"/>
     </row>
     <row r="94" spans="1:7" ht="109.05" customHeight="1">
       <c r="A94" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B94" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C94" s="22"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="22"/>
-      <c r="G94" s="23"/>
+      <c r="B94" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C94" s="23"/>
+      <c r="D94" s="23"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="23"/>
+      <c r="G94" s="24"/>
     </row>
     <row r="95" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A95" s="24" t="s">
+      <c r="A95" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B95" s="27"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="28"/>
-      <c r="E95" s="28"/>
-      <c r="F95" s="28"/>
-      <c r="G95" s="29"/>
+      <c r="B95" s="28"/>
+      <c r="C95" s="29"/>
+      <c r="D95" s="29"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="29"/>
+      <c r="G95" s="30"/>
     </row>
     <row r="96" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A96" s="25"/>
-      <c r="B96" s="30"/>
-      <c r="C96" s="31"/>
-      <c r="D96" s="31"/>
-      <c r="E96" s="31"/>
-      <c r="F96" s="31"/>
-      <c r="G96" s="32"/>
+      <c r="A96" s="26"/>
+      <c r="B96" s="31"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="32"/>
+      <c r="E96" s="32"/>
+      <c r="F96" s="32"/>
+      <c r="G96" s="33"/>
     </row>
     <row r="97" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A97" s="25"/>
-      <c r="B97" s="30"/>
-      <c r="C97" s="31"/>
-      <c r="D97" s="31"/>
-      <c r="E97" s="31"/>
-      <c r="F97" s="31"/>
-      <c r="G97" s="32"/>
+      <c r="A97" s="26"/>
+      <c r="B97" s="31"/>
+      <c r="C97" s="32"/>
+      <c r="D97" s="32"/>
+      <c r="E97" s="32"/>
+      <c r="F97" s="32"/>
+      <c r="G97" s="33"/>
     </row>
     <row r="98" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A98" s="26"/>
-      <c r="B98" s="33"/>
-      <c r="C98" s="34"/>
-      <c r="D98" s="34"/>
-      <c r="E98" s="34"/>
-      <c r="F98" s="34"/>
-      <c r="G98" s="35"/>
+      <c r="A98" s="27"/>
+      <c r="B98" s="34"/>
+      <c r="C98" s="35"/>
+      <c r="D98" s="35"/>
+      <c r="E98" s="35"/>
+      <c r="F98" s="35"/>
+      <c r="G98" s="36"/>
     </row>
     <row r="99" spans="1:7" ht="109.05" customHeight="1">
       <c r="A99" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B99" s="14"/>
-      <c r="C99" s="15"/>
-      <c r="D99" s="15"/>
-      <c r="E99" s="15"/>
-      <c r="F99" s="15"/>
-      <c r="G99" s="16"/>
+      <c r="B99" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C99" s="16"/>
+      <c r="D99" s="16"/>
+      <c r="E99" s="16"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="17"/>
     </row>
     <row r="101" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A101" s="17" t="s">
+      <c r="A101" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B101" s="18"/>
-      <c r="C101" s="18"/>
-      <c r="D101" s="18"/>
-      <c r="E101" s="18"/>
-      <c r="F101" s="18"/>
-      <c r="G101" s="19"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="19"/>
+      <c r="G101" s="20"/>
     </row>
     <row r="102" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A102" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B102" s="18"/>
-      <c r="C102" s="18"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="18"/>
-      <c r="G102" s="19"/>
+      <c r="A102" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B102" s="19"/>
+      <c r="C102" s="19"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="19"/>
+      <c r="G102" s="20"/>
     </row>
     <row r="103" spans="1:7" ht="109.05" customHeight="1">
       <c r="A103" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B103" s="21"/>
-      <c r="C103" s="22"/>
-      <c r="D103" s="22"/>
-      <c r="E103" s="22"/>
-      <c r="F103" s="22"/>
-      <c r="G103" s="23"/>
+      <c r="B103" s="22"/>
+      <c r="C103" s="23"/>
+      <c r="D103" s="23"/>
+      <c r="E103" s="23"/>
+      <c r="F103" s="23"/>
+      <c r="G103" s="24"/>
     </row>
     <row r="104" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A104" s="24" t="s">
+      <c r="A104" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B104" s="27"/>
-      <c r="C104" s="28"/>
-      <c r="D104" s="28"/>
-      <c r="E104" s="28"/>
-      <c r="F104" s="28"/>
-      <c r="G104" s="29"/>
+      <c r="B104" s="28"/>
+      <c r="C104" s="29"/>
+      <c r="D104" s="29"/>
+      <c r="E104" s="29"/>
+      <c r="F104" s="29"/>
+      <c r="G104" s="30"/>
     </row>
     <row r="105" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A105" s="25"/>
-      <c r="B105" s="30"/>
-      <c r="C105" s="31"/>
-      <c r="D105" s="31"/>
-      <c r="E105" s="31"/>
-      <c r="F105" s="31"/>
-      <c r="G105" s="32"/>
+      <c r="A105" s="26"/>
+      <c r="B105" s="31"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="32"/>
+      <c r="E105" s="32"/>
+      <c r="F105" s="32"/>
+      <c r="G105" s="33"/>
     </row>
     <row r="106" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A106" s="25"/>
-      <c r="B106" s="30"/>
-      <c r="C106" s="31"/>
-      <c r="D106" s="31"/>
-      <c r="E106" s="31"/>
-      <c r="F106" s="31"/>
-      <c r="G106" s="32"/>
+      <c r="A106" s="26"/>
+      <c r="B106" s="31"/>
+      <c r="C106" s="32"/>
+      <c r="D106" s="32"/>
+      <c r="E106" s="32"/>
+      <c r="F106" s="32"/>
+      <c r="G106" s="33"/>
     </row>
     <row r="107" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A107" s="26"/>
-      <c r="B107" s="33"/>
-      <c r="C107" s="34"/>
-      <c r="D107" s="34"/>
-      <c r="E107" s="34"/>
-      <c r="F107" s="34"/>
-      <c r="G107" s="35"/>
+      <c r="A107" s="27"/>
+      <c r="B107" s="34"/>
+      <c r="C107" s="35"/>
+      <c r="D107" s="35"/>
+      <c r="E107" s="35"/>
+      <c r="F107" s="35"/>
+      <c r="G107" s="36"/>
     </row>
     <row r="108" spans="1:7" ht="109.05" customHeight="1">
       <c r="A108" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B108" s="14"/>
-      <c r="C108" s="15"/>
-      <c r="D108" s="15"/>
-      <c r="E108" s="15"/>
-      <c r="F108" s="15"/>
-      <c r="G108" s="16"/>
+      <c r="B108" s="15"/>
+      <c r="C108" s="16"/>
+      <c r="D108" s="16"/>
+      <c r="E108" s="16"/>
+      <c r="F108" s="16"/>
+      <c r="G108" s="17"/>
     </row>
     <row r="110" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A110" s="17"/>
-      <c r="B110" s="18"/>
-      <c r="C110" s="18"/>
-      <c r="D110" s="18"/>
-      <c r="E110" s="18"/>
-      <c r="F110" s="18"/>
-      <c r="G110" s="19"/>
+      <c r="A110" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B110" s="19"/>
+      <c r="C110" s="19"/>
+      <c r="D110" s="19"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="20"/>
     </row>
     <row r="111" spans="1:7" ht="28.05" customHeight="1">
-      <c r="A111" s="20"/>
-      <c r="B111" s="18"/>
-      <c r="C111" s="18"/>
-      <c r="D111" s="18"/>
-      <c r="E111" s="18"/>
-      <c r="F111" s="18"/>
-      <c r="G111" s="19"/>
-    </row>
-    <row r="112" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A112" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B112" s="21"/>
-      <c r="C112" s="22"/>
-      <c r="D112" s="22"/>
-      <c r="E112" s="22"/>
-      <c r="F112" s="22"/>
-      <c r="G112" s="23"/>
+      <c r="A111" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B111" s="19"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="19"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="20"/>
+    </row>
+    <row r="112" spans="1:7" ht="177.6" customHeight="1">
+      <c r="A112" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B112" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C112" s="35"/>
+      <c r="D112" s="35"/>
+      <c r="E112" s="35"/>
+      <c r="F112" s="35"/>
+      <c r="G112" s="36"/>
     </row>
     <row r="113" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A113" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B113" s="27"/>
-      <c r="C113" s="28"/>
-      <c r="D113" s="28"/>
-      <c r="E113" s="28"/>
-      <c r="F113" s="28"/>
-      <c r="G113" s="29"/>
-    </row>
-    <row r="114" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A114" s="25"/>
-      <c r="B114" s="30"/>
-      <c r="C114" s="31"/>
-      <c r="D114" s="31"/>
-      <c r="E114" s="31"/>
-      <c r="F114" s="31"/>
-      <c r="G114" s="32"/>
-    </row>
-    <row r="115" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A115" s="25"/>
-      <c r="B115" s="30"/>
-      <c r="C115" s="31"/>
-      <c r="D115" s="31"/>
-      <c r="E115" s="31"/>
-      <c r="F115" s="31"/>
-      <c r="G115" s="32"/>
-    </row>
-    <row r="116" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A116" s="26"/>
-      <c r="B116" s="33"/>
-      <c r="C116" s="34"/>
-      <c r="D116" s="34"/>
-      <c r="E116" s="34"/>
-      <c r="F116" s="34"/>
-      <c r="G116" s="35"/>
-    </row>
-    <row r="117" spans="1:7" ht="109.05" customHeight="1">
-      <c r="A117" s="2" t="s">
+      <c r="A113" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B117" s="14"/>
-      <c r="C117" s="15"/>
-      <c r="D117" s="15"/>
-      <c r="E117" s="15"/>
-      <c r="F117" s="15"/>
-      <c r="G117" s="16"/>
+      <c r="B113" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C113" s="16"/>
+      <c r="D113" s="16"/>
+      <c r="E113" s="16"/>
+      <c r="F113" s="16"/>
+      <c r="G113" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="86">
+  <mergeCells count="84">
     <mergeCell ref="B54:G54"/>
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="B59:G62"/>
@@ -2435,11 +2425,6 @@
     <mergeCell ref="A12:G12"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G17"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="A16:A17"/>
     <mergeCell ref="B32:G35"/>
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="A30:G30"/>
@@ -2451,6 +2436,11 @@
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="B16:G17"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="B72:G72"/>
     <mergeCell ref="B63:G63"/>
     <mergeCell ref="A65:G65"/>
@@ -2480,13 +2470,11 @@
     <mergeCell ref="B103:G103"/>
     <mergeCell ref="A104:A107"/>
     <mergeCell ref="B104:G107"/>
-    <mergeCell ref="B117:G117"/>
+    <mergeCell ref="B113:G113"/>
     <mergeCell ref="B108:G108"/>
     <mergeCell ref="A110:G110"/>
     <mergeCell ref="A111:G111"/>
     <mergeCell ref="B112:G112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="B113:G116"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A48" r:id="rId1" xr:uid="{E9CA4E32-E474-DC42-91CA-A034567F6E87}"/>
@@ -2501,8 +2489,9 @@
     <hyperlink ref="A84" r:id="rId10" xr:uid="{356F7947-C64D-2A4D-AAFD-DE87C3693791}"/>
     <hyperlink ref="A93" r:id="rId11" xr:uid="{EA0DFB72-F906-4DF0-9671-3FA386C9320A}"/>
     <hyperlink ref="A102" r:id="rId12" xr:uid="{82D1E942-7322-42D7-ABDF-C0104BD1FEF8}"/>
+    <hyperlink ref="A111" r:id="rId13" xr:uid="{0A762ADB-859A-4560-A659-AAB21AC72186}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Work Blockchain Notes.xlsx
</commit_message>
<xml_diff>
--- a/Work Blockchain Notes.xlsx
+++ b/Work Blockchain Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Work\blockchaining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD061BFE-C8EA-4428-8B0E-3CADB8F17822}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0870DB6F-0979-40D8-9297-D6576A7DE0C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22950" yWindow="8700" windowWidth="23040" windowHeight="12210" xr2:uid="{BDE38765-44BC-5F4C-A678-8771D11B51DC}"/>
+    <workbookView xWindow="29895" yWindow="9300" windowWidth="18435" windowHeight="9765" xr2:uid="{BDE38765-44BC-5F4C-A678-8771D11B51DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="101">
   <si>
     <t>Abstract</t>
   </si>
@@ -328,6 +328,21 @@
   </si>
   <si>
     <t>Yes, I know, it's another YouTube video, but it's how I'm getting up to speed on Ethereum and the Ethereum Virtual Machine used to write Solidity</t>
+  </si>
+  <si>
+    <t>https://www.accenture-insights.nl/en-us/articles/blockchain-aircraft-spare-part-tracking-impact-mros</t>
+  </si>
+  <si>
+    <t>Using blockchain for aircraft spare parts tracking: impact on MROs</t>
+  </si>
+  <si>
+    <t>While not a research paper or a scholarly journal, this article is pretty close to what we're looking for</t>
+  </si>
+  <si>
+    <t>Talks a lot about spare part tracking using blockchain to track components. Still doesn't tell us a lot technically, but it does discuss the benefits blockchain offers in this field</t>
+  </si>
+  <si>
+    <t>Seems relevant to me</t>
   </si>
 </sst>
 </file>
@@ -882,14 +897,62 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -897,48 +960,81 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -950,87 +1046,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1061,7 +1076,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1346834</xdr:colOff>
+      <xdr:colOff>1354454</xdr:colOff>
       <xdr:row>100</xdr:row>
       <xdr:rowOff>269691</xdr:rowOff>
     </xdr:to>
@@ -1395,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659183C7-6FCE-A94E-ACE3-15A5F17A3D83}">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106:G106"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -1407,412 +1422,412 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:7" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:7" ht="121.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:7" ht="176.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:7" ht="91.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="1:7" ht="91.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
     </row>
     <row r="8" spans="1:7" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="45"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="25"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
     </row>
     <row r="13" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:7" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="1:7" ht="210" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
     </row>
     <row r="18" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="21"/>
     </row>
     <row r="20" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
     </row>
     <row r="21" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="31"/>
     </row>
     <row r="22" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="31"/>
     </row>
     <row r="23" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="31"/>
     </row>
     <row r="24" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="45"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="28"/>
     </row>
     <row r="25" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="1:7" ht="28.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="41"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="56"/>
     </row>
     <row r="27" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="38"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="53"/>
     </row>
     <row r="28" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="33"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="60"/>
     </row>
     <row r="29" spans="1:7" ht="385.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="42"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
     </row>
     <row r="30" spans="1:7" ht="109.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="36"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="63"/>
     </row>
     <row r="31" spans="1:7" ht="42" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="46"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="47"/>
+      <c r="G31" s="15"/>
     </row>
     <row r="32" spans="1:7" ht="28.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="49"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="50"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="45"/>
     </row>
     <row r="33" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="52"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="47"/>
     </row>
     <row r="34" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="53" t="s">
+      <c r="A34" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="54"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="42"/>
     </row>
     <row r="35" spans="1:7" ht="282.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="54"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="42"/>
     </row>
     <row r="36" spans="1:7" ht="109.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="55" t="s">
+      <c r="A36" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="58"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="59"/>
     </row>
     <row r="37" spans="1:7" ht="28.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
@@ -1824,65 +1839,65 @@
       <c r="G37" s="6"/>
     </row>
     <row r="38" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="25"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="21"/>
     </row>
     <row r="39" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="25"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="21"/>
     </row>
     <row r="40" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="29"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="31"/>
     </row>
     <row r="41" spans="1:7" ht="272.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="32"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="41"/>
     </row>
     <row r="42" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="16"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="51"/>
     </row>
     <row r="43" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
@@ -1894,669 +1909,771 @@
       <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="25"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="21"/>
     </row>
     <row r="45" spans="1:7" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="25"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="21"/>
     </row>
     <row r="46" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="29"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="31"/>
     </row>
     <row r="47" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="32"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="41"/>
     </row>
     <row r="48" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="45"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="28"/>
     </row>
     <row r="50" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="23" t="s">
+      <c r="A50" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="25"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="21"/>
     </row>
     <row r="51" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="25"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="21"/>
     </row>
     <row r="52" spans="1:7" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="29"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="31"/>
     </row>
     <row r="53" spans="1:7" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="27" t="s">
+      <c r="B53" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="29"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="31"/>
     </row>
     <row r="54" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="16"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="51"/>
     </row>
     <row r="55" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="56" spans="1:7" ht="28.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="48" t="s">
+      <c r="A56" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="49"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="49"/>
-      <c r="G56" s="50"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="45"/>
     </row>
     <row r="57" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="51" t="s">
+      <c r="A57" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="52"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="47"/>
     </row>
     <row r="58" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="59" t="s">
+      <c r="A58" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="27" t="s">
+      <c r="B58" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="54"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="42"/>
     </row>
     <row r="59" spans="1:7" ht="232.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="53" t="s">
+      <c r="A59" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B59" s="27" t="s">
+      <c r="B59" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="28"/>
-      <c r="F59" s="28"/>
-      <c r="G59" s="54"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="42"/>
     </row>
     <row r="60" spans="1:7" ht="109.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="55" t="s">
+      <c r="A60" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B60" s="60" t="s">
+      <c r="B60" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="C60" s="61"/>
-      <c r="D60" s="61"/>
-      <c r="E60" s="61"/>
-      <c r="F60" s="61"/>
-      <c r="G60" s="62"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="40"/>
     </row>
     <row r="61" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="23" t="s">
+      <c r="A62" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="25"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="21"/>
     </row>
     <row r="63" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="26" t="s">
+      <c r="A63" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="24"/>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="25"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="21"/>
     </row>
     <row r="64" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B64" s="27" t="s">
+      <c r="B64" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C64" s="28"/>
-      <c r="D64" s="28"/>
-      <c r="E64" s="28"/>
-      <c r="F64" s="28"/>
-      <c r="G64" s="29"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="31"/>
     </row>
     <row r="65" spans="1:7" ht="234.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B65" s="27"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="28"/>
-      <c r="E65" s="28"/>
-      <c r="F65" s="28"/>
-      <c r="G65" s="29"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="31"/>
     </row>
     <row r="66" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="44"/>
-      <c r="D66" s="44"/>
-      <c r="E66" s="44"/>
-      <c r="F66" s="44"/>
-      <c r="G66" s="45"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="28"/>
     </row>
     <row r="68" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="23" t="s">
+      <c r="A68" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="25"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="21"/>
     </row>
     <row r="69" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="26" t="s">
+      <c r="A69" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B69" s="24"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="25"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="21"/>
     </row>
     <row r="70" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B70" s="27" t="s">
+      <c r="B70" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="28"/>
-      <c r="F70" s="28"/>
-      <c r="G70" s="29"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="30"/>
+      <c r="F70" s="30"/>
+      <c r="G70" s="31"/>
     </row>
     <row r="71" spans="1:7" ht="217.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B71" s="27"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="28"/>
-      <c r="G71" s="29"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="31"/>
     </row>
     <row r="72" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B72" s="43" t="s">
+      <c r="B72" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C72" s="44"/>
-      <c r="D72" s="44"/>
-      <c r="E72" s="44"/>
-      <c r="F72" s="44"/>
-      <c r="G72" s="45"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="28"/>
     </row>
     <row r="74" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="23" t="s">
+      <c r="A74" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B74" s="24"/>
-      <c r="C74" s="24"/>
-      <c r="D74" s="24"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="25"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="21"/>
     </row>
     <row r="75" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="26" t="s">
+      <c r="A75" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B75" s="24"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="24"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="25"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="21"/>
     </row>
     <row r="76" spans="1:7" ht="177.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B76" s="20" t="s">
+      <c r="B76" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C76" s="21"/>
-      <c r="D76" s="21"/>
-      <c r="E76" s="21"/>
-      <c r="F76" s="21"/>
-      <c r="G76" s="22"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="25"/>
     </row>
     <row r="77" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B77" s="43" t="s">
+      <c r="B77" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C77" s="44"/>
-      <c r="D77" s="44"/>
-      <c r="E77" s="44"/>
-      <c r="F77" s="44"/>
-      <c r="G77" s="45"/>
+      <c r="C77" s="27"/>
+      <c r="D77" s="27"/>
+      <c r="E77" s="27"/>
+      <c r="F77" s="27"/>
+      <c r="G77" s="28"/>
     </row>
     <row r="78" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="79" spans="1:7" ht="28.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="48" t="s">
+      <c r="A79" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B79" s="49"/>
-      <c r="C79" s="49"/>
-      <c r="D79" s="49"/>
-      <c r="E79" s="49"/>
-      <c r="F79" s="49"/>
-      <c r="G79" s="50"/>
+      <c r="B79" s="44"/>
+      <c r="C79" s="44"/>
+      <c r="D79" s="44"/>
+      <c r="E79" s="44"/>
+      <c r="F79" s="44"/>
+      <c r="G79" s="45"/>
     </row>
     <row r="80" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="51" t="s">
+      <c r="A80" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="B80" s="24"/>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24"/>
-      <c r="G80" s="52"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="47"/>
     </row>
     <row r="81" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="59" t="s">
+      <c r="A81" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="27" t="s">
+      <c r="B81" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="28"/>
-      <c r="F81" s="28"/>
-      <c r="G81" s="54"/>
+      <c r="C81" s="30"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="30"/>
+      <c r="F81" s="30"/>
+      <c r="G81" s="42"/>
     </row>
     <row r="82" spans="1:7" ht="343.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="53" t="s">
+      <c r="A82" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B82" s="19" t="s">
+      <c r="B82" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C82" s="17"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="17"/>
-      <c r="F82" s="17"/>
-      <c r="G82" s="63"/>
+      <c r="C82" s="33"/>
+      <c r="D82" s="33"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="33"/>
+      <c r="G82" s="48"/>
     </row>
     <row r="83" spans="1:7" ht="109.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="55" t="s">
+      <c r="A83" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="60" t="s">
+      <c r="B83" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C83" s="61"/>
-      <c r="D83" s="61"/>
-      <c r="E83" s="61"/>
-      <c r="F83" s="61"/>
-      <c r="G83" s="62"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
+      <c r="E83" s="39"/>
+      <c r="F83" s="39"/>
+      <c r="G83" s="40"/>
     </row>
     <row r="84" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="23" t="s">
+      <c r="A85" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B85" s="24"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="25"/>
+      <c r="B85" s="20"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="21"/>
     </row>
     <row r="86" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="26" t="s">
+      <c r="A86" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B86" s="24"/>
-      <c r="C86" s="24"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24"/>
-      <c r="G86" s="25"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="20"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="21"/>
     </row>
     <row r="87" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B87" s="27" t="s">
+      <c r="B87" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="C87" s="28"/>
-      <c r="D87" s="28"/>
-      <c r="E87" s="28"/>
-      <c r="F87" s="28"/>
-      <c r="G87" s="29"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="30"/>
+      <c r="G87" s="31"/>
     </row>
     <row r="88" spans="1:7" ht="343.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B88" s="19" t="s">
+      <c r="B88" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="C88" s="17"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="17"/>
-      <c r="G88" s="18"/>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="34"/>
     </row>
     <row r="89" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B89" s="43" t="s">
+      <c r="B89" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C89" s="44"/>
-      <c r="D89" s="44"/>
-      <c r="E89" s="44"/>
-      <c r="F89" s="44"/>
-      <c r="G89" s="45"/>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
+      <c r="E89" s="27"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="28"/>
     </row>
     <row r="91" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="23" t="s">
+      <c r="A91" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B91" s="24"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="25"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="20"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="21"/>
     </row>
     <row r="92" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="26" t="s">
+      <c r="A92" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B92" s="24"/>
-      <c r="C92" s="24"/>
-      <c r="D92" s="24"/>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
-      <c r="G92" s="25"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="20"/>
+      <c r="D92" s="20"/>
+      <c r="E92" s="20"/>
+      <c r="F92" s="20"/>
+      <c r="G92" s="21"/>
     </row>
     <row r="93" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="27" t="s">
+      <c r="B93" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="C93" s="28"/>
-      <c r="D93" s="28"/>
-      <c r="E93" s="28"/>
-      <c r="F93" s="28"/>
-      <c r="G93" s="29"/>
+      <c r="C93" s="30"/>
+      <c r="D93" s="30"/>
+      <c r="E93" s="30"/>
+      <c r="F93" s="30"/>
+      <c r="G93" s="31"/>
     </row>
     <row r="94" spans="1:7" ht="343.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B94" s="19" t="s">
+      <c r="B94" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="C94" s="17"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="17"/>
-      <c r="F94" s="17"/>
-      <c r="G94" s="18"/>
+      <c r="C94" s="33"/>
+      <c r="D94" s="33"/>
+      <c r="E94" s="33"/>
+      <c r="F94" s="33"/>
+      <c r="G94" s="34"/>
     </row>
     <row r="95" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B95" s="43" t="s">
+      <c r="B95" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C95" s="44"/>
-      <c r="D95" s="44"/>
-      <c r="E95" s="44"/>
-      <c r="F95" s="44"/>
-      <c r="G95" s="45"/>
+      <c r="C95" s="27"/>
+      <c r="D95" s="27"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="27"/>
+      <c r="G95" s="28"/>
     </row>
     <row r="97" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="23" t="s">
+      <c r="A97" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B97" s="24"/>
-      <c r="C97" s="24"/>
-      <c r="D97" s="24"/>
-      <c r="E97" s="24"/>
-      <c r="F97" s="24"/>
-      <c r="G97" s="25"/>
+      <c r="B97" s="20"/>
+      <c r="C97" s="20"/>
+      <c r="D97" s="20"/>
+      <c r="E97" s="20"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="21"/>
     </row>
     <row r="98" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="26" t="s">
+      <c r="A98" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B98" s="24"/>
-      <c r="C98" s="24"/>
-      <c r="D98" s="24"/>
-      <c r="E98" s="24"/>
-      <c r="F98" s="24"/>
-      <c r="G98" s="25"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="20"/>
+      <c r="G98" s="21"/>
     </row>
     <row r="99" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B99" s="27" t="s">
+      <c r="B99" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C99" s="28"/>
-      <c r="D99" s="28"/>
-      <c r="E99" s="28"/>
-      <c r="F99" s="28"/>
-      <c r="G99" s="29"/>
+      <c r="C99" s="30"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="30"/>
+      <c r="F99" s="30"/>
+      <c r="G99" s="31"/>
     </row>
     <row r="100" spans="1:7" ht="343.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B100" s="19" t="s">
+      <c r="B100" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C100" s="17"/>
-      <c r="D100" s="17"/>
-      <c r="E100" s="17"/>
-      <c r="F100" s="17"/>
-      <c r="G100" s="18"/>
+      <c r="C100" s="33"/>
+      <c r="D100" s="33"/>
+      <c r="E100" s="33"/>
+      <c r="F100" s="33"/>
+      <c r="G100" s="34"/>
     </row>
     <row r="101" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B101" s="43" t="s">
+      <c r="B101" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C101" s="44"/>
-      <c r="D101" s="44"/>
-      <c r="E101" s="44"/>
-      <c r="F101" s="44"/>
-      <c r="G101" s="45"/>
+      <c r="C101" s="27"/>
+      <c r="D101" s="27"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="27"/>
+      <c r="G101" s="28"/>
     </row>
     <row r="103" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="23" t="s">
+      <c r="A103" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B103" s="24"/>
-      <c r="C103" s="24"/>
-      <c r="D103" s="24"/>
-      <c r="E103" s="24"/>
-      <c r="F103" s="24"/>
-      <c r="G103" s="25"/>
+      <c r="B103" s="20"/>
+      <c r="C103" s="20"/>
+      <c r="D103" s="20"/>
+      <c r="E103" s="20"/>
+      <c r="F103" s="20"/>
+      <c r="G103" s="21"/>
     </row>
     <row r="104" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="26" t="s">
+      <c r="A104" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B104" s="24"/>
-      <c r="C104" s="24"/>
-      <c r="D104" s="24"/>
-      <c r="E104" s="24"/>
-      <c r="F104" s="24"/>
-      <c r="G104" s="25"/>
+      <c r="B104" s="20"/>
+      <c r="C104" s="20"/>
+      <c r="D104" s="20"/>
+      <c r="E104" s="20"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="21"/>
     </row>
     <row r="105" spans="1:7" ht="177.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B105" s="20" t="s">
+      <c r="B105" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C105" s="21"/>
-      <c r="D105" s="21"/>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
-      <c r="G105" s="22"/>
+      <c r="C105" s="24"/>
+      <c r="D105" s="24"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="25"/>
     </row>
     <row r="106" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B106" s="43" t="s">
+      <c r="B106" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C106" s="44"/>
-      <c r="D106" s="44"/>
-      <c r="E106" s="44"/>
-      <c r="F106" s="44"/>
-      <c r="G106" s="45"/>
+      <c r="C106" s="27"/>
+      <c r="D106" s="27"/>
+      <c r="E106" s="27"/>
+      <c r="F106" s="27"/>
+      <c r="G106" s="28"/>
+    </row>
+    <row r="108" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B108" s="20"/>
+      <c r="C108" s="20"/>
+      <c r="D108" s="20"/>
+      <c r="E108" s="20"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="21"/>
+    </row>
+    <row r="109" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B109" s="20"/>
+      <c r="C109" s="20"/>
+      <c r="D109" s="20"/>
+      <c r="E109" s="20"/>
+      <c r="F109" s="20"/>
+      <c r="G109" s="21"/>
+    </row>
+    <row r="110" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C110" s="30"/>
+      <c r="D110" s="30"/>
+      <c r="E110" s="30"/>
+      <c r="F110" s="30"/>
+      <c r="G110" s="31"/>
+    </row>
+    <row r="111" spans="1:7" ht="262.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B111" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C111" s="33"/>
+      <c r="D111" s="33"/>
+      <c r="E111" s="33"/>
+      <c r="F111" s="33"/>
+      <c r="G111" s="34"/>
+    </row>
+    <row r="112" spans="1:7" ht="109.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C112" s="27"/>
+      <c r="D112" s="27"/>
+      <c r="E112" s="27"/>
+      <c r="F112" s="27"/>
+      <c r="G112" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="90">
-    <mergeCell ref="A103:G103"/>
-    <mergeCell ref="A104:G104"/>
-    <mergeCell ref="B105:G105"/>
-    <mergeCell ref="B106:G106"/>
-    <mergeCell ref="A97:G97"/>
-    <mergeCell ref="A98:G98"/>
-    <mergeCell ref="B99:G99"/>
-    <mergeCell ref="B100:G100"/>
-    <mergeCell ref="B101:G101"/>
-    <mergeCell ref="A91:G91"/>
-    <mergeCell ref="A92:G92"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="B94:G94"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="A85:G85"/>
-    <mergeCell ref="A86:G86"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="B88:G88"/>
-    <mergeCell ref="B89:G89"/>
+  <mergeCells count="95">
+    <mergeCell ref="B111:G111"/>
+    <mergeCell ref="B112:G112"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="A108:G108"/>
+    <mergeCell ref="A109:G109"/>
+    <mergeCell ref="B110:G110"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="A44:G44"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="A57:G57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B66:G66"/>
+    <mergeCell ref="A68:G68"/>
+    <mergeCell ref="A69:G69"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="A62:G62"/>
+    <mergeCell ref="A63:G63"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="A75:G75"/>
+    <mergeCell ref="B76:G76"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="B15:G15"/>
@@ -2573,61 +2690,25 @@
     <mergeCell ref="A80:G80"/>
     <mergeCell ref="B81:G81"/>
     <mergeCell ref="B82:G82"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="A75:G75"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="A68:G68"/>
-    <mergeCell ref="A69:G69"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="A62:G62"/>
-    <mergeCell ref="A63:G63"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="A57:G57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="A85:G85"/>
+    <mergeCell ref="A86:G86"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="B88:G88"/>
+    <mergeCell ref="B89:G89"/>
+    <mergeCell ref="A91:G91"/>
+    <mergeCell ref="A92:G92"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="B94:G94"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="A103:G103"/>
+    <mergeCell ref="A104:G104"/>
+    <mergeCell ref="B105:G105"/>
+    <mergeCell ref="B106:G106"/>
+    <mergeCell ref="A97:G97"/>
+    <mergeCell ref="A98:G98"/>
+    <mergeCell ref="B99:G99"/>
+    <mergeCell ref="B100:G100"/>
+    <mergeCell ref="B101:G101"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A39" r:id="rId1" xr:uid="{E9CA4E32-E474-DC42-91CA-A034567F6E87}"/>
@@ -2647,9 +2728,10 @@
     <hyperlink ref="A98" r:id="rId15" xr:uid="{34FF6B2E-D511-4F3D-B262-1C966FE9C3B9}"/>
     <hyperlink ref="A92" r:id="rId16" xr:uid="{7B9A8902-EC40-464D-9B8B-D694E6E511FB}"/>
     <hyperlink ref="A104" r:id="rId17" xr:uid="{D11FD2BD-B0AC-48E3-9E23-33D77133ADAC}"/>
+    <hyperlink ref="A109" r:id="rId18" xr:uid="{58719267-092C-42B9-9E3D-50D22169C7C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
-  <drawing r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>